<commit_message>
penambahan export komisi harian dan tahunan
</commit_message>
<xml_diff>
--- a/datakomisigrobulanan.xlsx
+++ b/datakomisigrobulanan.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,9 +476,9 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="33.6" customWidth="1" min="4" max="4"/>
+    <col width="16.8" customWidth="1" min="4" max="4"/>
     <col width="15.6" customWidth="1" min="5" max="5"/>
-    <col width="10.8" customWidth="1" min="6" max="6"/>
+    <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
     <col width="10.8" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
   </cols>
@@ -500,7 +500,7 @@
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>LAPORAN KOMISI GRO BULAN 7 TAHUN 2025</t>
+          <t>LAPORAN KOMISI GRO BULAN 6 TAHUN 2025</t>
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
@@ -557,7 +557,7 @@
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>Terapis :</t>
+          <t>Gro :</t>
         </is>
       </c>
       <c r="B5" s="6" t="inlineStr">
@@ -575,22 +575,22 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>TF0091</t>
+          <t>TF0068</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>06-07-2025 15:28:18</t>
+          <t>15-06-2025 14:33:27</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>P003</t>
+          <t>M019</t>
         </is>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>Hot Stone</t>
+          <t>Paket Jamail</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
@@ -599,11 +599,11 @@
         </is>
       </c>
       <c r="F6" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>35.000</t>
+          <t>70.000</t>
         </is>
       </c>
       <c r="H6" s="6" t="inlineStr">
@@ -615,27 +615,27 @@
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>TF0091</t>
+          <t>TF0069</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>06-07-2025 15:28:18</t>
+          <t>15-06-2025 14:35:15</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>P001</t>
+          <t>M019</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>Traditional Massage 30 Min</t>
+          <t>Paket Jamail</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>200.000</t>
+          <t>350.000</t>
         </is>
       </c>
       <c r="F7" s="8" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>10.000</t>
+          <t>70.000</t>
         </is>
       </c>
       <c r="H7" s="6" t="inlineStr">
@@ -655,12 +655,12 @@
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>TF0091</t>
+          <t>TF0071</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>06-07-2025 15:28:18</t>
+          <t>15-06-2025 14:46:23</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
@@ -679,11 +679,11 @@
         </is>
       </c>
       <c r="F8" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="7" t="inlineStr">
         <is>
-          <t>140.000</t>
+          <t>70.000</t>
         </is>
       </c>
       <c r="H8" s="6" t="inlineStr">
@@ -693,46 +693,286 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>TF0073</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 14:52:39</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H9" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>TF0074</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 15:05:29</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H10" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>TF0075</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 15:09:27</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H11" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>TF0076</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 15:13:13</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H12" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>TF0077</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 15:14:34</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H13" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>TF0083</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>15-06-2025 18:27:47</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>M019</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>Paket Jamail</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>350.000</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="inlineStr">
+        <is>
+          <t>70.000</t>
+        </is>
+      </c>
+      <c r="H14" s="6" t="inlineStr">
+        <is>
+          <t>Sdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B9" s="6" t="n"/>
-      <c r="C9" s="6" t="n"/>
-      <c r="D9" s="6" t="n"/>
-      <c r="E9" s="6" t="n"/>
-      <c r="F9" s="10" t="inlineStr">
-        <is>
-          <t>185.000</t>
-        </is>
-      </c>
-      <c r="G9" s="9" t="inlineStr"/>
-      <c r="H9" s="9" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="inlineStr">
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
+      <c r="D15" s="6" t="n"/>
+      <c r="E15" s="6" t="n"/>
+      <c r="F15" s="10" t="inlineStr"/>
+      <c r="G15" s="9" t="inlineStr">
+        <is>
+          <t>630.000</t>
+        </is>
+      </c>
+      <c r="H15" s="9" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>TOTAL SELURUH KOMISI</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n"/>
-      <c r="C12" s="5" t="inlineStr"/>
-      <c r="D12" s="5" t="inlineStr"/>
-      <c r="E12" s="5" t="inlineStr"/>
-      <c r="F12" s="5" t="inlineStr"/>
-      <c r="G12" s="5" t="inlineStr">
-        <is>
-          <t>185.000</t>
-        </is>
-      </c>
-      <c r="H12" s="11" t="n"/>
+      <c r="B18" s="5" t="n"/>
+      <c r="C18" s="5" t="inlineStr"/>
+      <c r="D18" s="5" t="inlineStr"/>
+      <c r="E18" s="5" t="inlineStr"/>
+      <c r="F18" s="5" t="inlineStr"/>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>630.000</t>
+        </is>
+      </c>
+      <c r="H18" s="11" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A15:E15"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>